<commit_message>
falls Leon noch was braucht anrufen
</commit_message>
<xml_diff>
--- a/Meilenstein 4/Dokumente/Stückliste_Drohne.xlsx
+++ b/Meilenstein 4/Dokumente/Stückliste_Drohne.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Methodisches Konstruieren\Übungen\git repo\MKon\Meilenstein 4\Dokumente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Birgi\OneDrive - haw-hamburg.de\Dokumente\GitHub\MKon\Meilenstein 4\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EE1042-72F3-4962-8C77-80B1442FEF45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B68BF95-D364-4C5F-991F-55910ED67B34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8629A93B-4D8D-4644-A0F5-A6E2E52E581F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8629A93B-4D8D-4644-A0F5-A6E2E52E581F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="97">
   <si>
     <t>Teil ID</t>
   </si>
@@ -855,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891C9133-3018-4E2B-9D85-939881835433}">
   <dimension ref="B3:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,8 +1076,8 @@
       <c r="B15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>94</v>
+      <c r="C15" s="14">
+        <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>52</v>
@@ -1263,8 +1263,8 @@
       <c r="B26" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>94</v>
+      <c r="C26" s="14">
+        <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>33</v>
@@ -1297,8 +1297,8 @@
       <c r="B28" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>94</v>
+      <c r="C28" s="14">
+        <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>35</v>
@@ -1331,8 +1331,8 @@
       <c r="B30" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>94</v>
+      <c r="C30" s="14">
+        <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>46</v>
@@ -1364,6 +1364,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>